<commit_message>
Chattahoochee completed, Severn started
</commit_message>
<xml_diff>
--- a/archived modeled files/Chattahoochee River/Dx_2017_Noori_et_al_Paper02_Chattahoochee.xlsx
+++ b/archived modeled files/Chattahoochee River/Dx_2017_Noori_et_al_Paper02_Chattahoochee.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="121">
   <si>
     <t>Project Name</t>
   </si>
@@ -416,9 +416,6 @@
     <t xml:space="preserve">Noori et al. (2017) </t>
   </si>
   <si>
-    <t>Li et al. 2 (1998)</t>
-  </si>
-  <si>
     <t>None Dispersive Model</t>
   </si>
   <si>
@@ -456,6 +453,21 @@
   </si>
   <si>
     <t>St7 @ 76.6 (km)</t>
+  </si>
+  <si>
+    <t>Li et al (1998)</t>
+  </si>
+  <si>
+    <t>Li et al 2 (1998)</t>
+  </si>
+  <si>
+    <t>Deng et al (2001)</t>
+  </si>
+  <si>
+    <t>Disley et al (2015)</t>
+  </si>
+  <si>
+    <t>Noori et al (2017)</t>
   </si>
 </sst>
 </file>
@@ -5444,7 +5456,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5486,7 +5498,7 @@
       </c>
       <c r="B2" s="42" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
-        <v>Dx_2017_Noori_et_al_Paper02_severn.xlsx</v>
+        <v>Dx_2017_Noori_et_al_Paper02_Chattahoochee.xlsx</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -5608,7 +5620,7 @@
       </c>
       <c r="B6" s="43" t="str">
         <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
-        <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\archived modeled files\Chattahoochee River\</v>
+        <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -5692,7 +5704,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="45">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -5722,7 +5734,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="66">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -5752,7 +5764,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -7961,7 +7973,7 @@
         <v>22</v>
       </c>
       <c r="X1" s="85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y1" s="86" t="s">
         <v>45</v>
@@ -8012,15 +8024,15 @@
         <v>81</v>
       </c>
       <c r="AO1" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP1" s="89" t="s">
         <v>106</v>
-      </c>
-      <c r="AP1" s="89" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:42" s="75" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="68">
         <v>0</v>
@@ -8099,11 +8111,11 @@
       </c>
       <c r="AB2" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1159</v>
+        <v>434</v>
       </c>
       <c r="AC2" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>266.66666666666669</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
@@ -8111,7 +8123,7 @@
       </c>
       <c r="AE2" s="75">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF2" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8131,7 +8143,7 @@
       </c>
       <c r="AJ2" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>10225.799999999999</v>
+        <v>17042.999999999996</v>
       </c>
       <c r="AK2" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8149,7 +8161,7 @@
       </c>
       <c r="AO2" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>266</v>
+        <v>160</v>
       </c>
       <c r="AP2" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8158,7 +8170,7 @@
     </row>
     <row r="3" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="68">
         <f>C2</f>
@@ -8238,19 +8250,19 @@
       </c>
       <c r="AB3" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1939</v>
+        <v>727</v>
       </c>
       <c r="AC3" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>465</v>
+        <v>279</v>
       </c>
       <c r="AD3" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>266.66666666666669</v>
+        <v>160</v>
       </c>
       <c r="AE3" s="75">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8270,7 +8282,7 @@
       </c>
       <c r="AJ3" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>11449.199999999999</v>
+        <v>19082</v>
       </c>
       <c r="AK3" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8288,7 +8300,7 @@
       </c>
       <c r="AO3" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>465</v>
+        <v>279</v>
       </c>
       <c r="AP3" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8297,7 +8309,7 @@
     </row>
     <row r="4" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="68">
         <f t="shared" ref="B4:B8" si="1">C3</f>
@@ -8377,19 +8389,19 @@
       </c>
       <c r="AB4" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>2479</v>
+        <v>929</v>
       </c>
       <c r="AC4" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>608.33333333333337</v>
+        <v>365</v>
       </c>
       <c r="AD4" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>465</v>
+        <v>279</v>
       </c>
       <c r="AE4" s="75">
         <f>Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF4" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8409,7 +8421,7 @@
       </c>
       <c r="AJ4" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>10225.799999999999</v>
+        <v>17042.999999999996</v>
       </c>
       <c r="AK4" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8423,7 +8435,7 @@
       <c r="AN4" s="75"/>
       <c r="AO4" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>608</v>
+        <v>365</v>
       </c>
       <c r="AP4" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8432,7 +8444,7 @@
     </row>
     <row r="5" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="68">
         <f t="shared" si="1"/>
@@ -8512,19 +8524,19 @@
       </c>
       <c r="AB5" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>3552</v>
+        <v>1332</v>
       </c>
       <c r="AC5" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>826.66666666666663</v>
+        <v>496</v>
       </c>
       <c r="AD5" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>608.33333333333337</v>
+        <v>365</v>
       </c>
       <c r="AE5" s="75">
         <f>Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF5" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8544,7 +8556,7 @@
       </c>
       <c r="AJ5" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>10722.599999999999</v>
+        <v>17870.999999999996</v>
       </c>
       <c r="AK5" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8558,7 +8570,7 @@
       <c r="AN5" s="75"/>
       <c r="AO5" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>826</v>
+        <v>496</v>
       </c>
       <c r="AP5" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8567,7 +8579,7 @@
     </row>
     <row r="6" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="68">
         <f t="shared" si="1"/>
@@ -8647,19 +8659,19 @@
       </c>
       <c r="AB6" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>4759</v>
+        <v>1784</v>
       </c>
       <c r="AC6" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>951.66666666666663</v>
+        <v>571</v>
       </c>
       <c r="AD6" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>826.66666666666663</v>
+        <v>496</v>
       </c>
       <c r="AE6" s="75">
         <f>Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF6" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8679,7 +8691,7 @@
       </c>
       <c r="AJ6" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>12196.8</v>
+        <v>20328</v>
       </c>
       <c r="AK6" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8693,7 +8705,7 @@
       <c r="AN6" s="75"/>
       <c r="AO6" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>951</v>
+        <v>571</v>
       </c>
       <c r="AP6" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8702,7 +8714,7 @@
     </row>
     <row r="7" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="80" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="68">
         <f t="shared" si="1"/>
@@ -8782,19 +8794,19 @@
       </c>
       <c r="AB7" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>5160</v>
+        <v>1935</v>
       </c>
       <c r="AC7" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>1008.3333333333334</v>
+        <v>605</v>
       </c>
       <c r="AD7" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>951.66666666666663</v>
+        <v>571</v>
       </c>
       <c r="AE7" s="75">
         <f>Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF7" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8814,7 +8826,7 @@
       </c>
       <c r="AJ7" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>12196.8</v>
+        <v>20328</v>
       </c>
       <c r="AK7" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8828,7 +8840,7 @@
       <c r="AN7" s="75"/>
       <c r="AO7" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>1008</v>
+        <v>605</v>
       </c>
       <c r="AP7" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8837,7 +8849,7 @@
     </row>
     <row r="8" spans="1:42" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="68">
         <f t="shared" si="1"/>
@@ -8917,19 +8929,19 @@
       </c>
       <c r="AB8" s="83">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>6916</v>
+        <v>2593</v>
       </c>
       <c r="AC8" s="83">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>1276.6666666666667</v>
+        <v>766</v>
       </c>
       <c r="AD8" s="83">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>1008.3333333333334</v>
+        <v>605</v>
       </c>
       <c r="AE8" s="75">
         <f>Delta_T__seconds</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AF8" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8949,7 +8961,7 @@
       </c>
       <c r="AJ8" s="82">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>9072</v>
+        <v>15119.999999999998</v>
       </c>
       <c r="AK8" s="82">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8963,7 +8975,7 @@
       <c r="AN8" s="75"/>
       <c r="AO8" s="79">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>1276</v>
+        <v>766</v>
       </c>
       <c r="AP8" s="79">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -9156,7 +9168,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="P2" sqref="P2:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9181,7 +9193,7 @@
         <v>5</v>
       </c>
       <c r="P2" s="59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9277,15 +9289,15 @@
         <v>350</v>
       </c>
       <c r="P11" s="60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12">
         <v>400</v>
       </c>
       <c r="P12" s="61" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9293,7 +9305,7 @@
         <v>450</v>
       </c>
       <c r="P13" s="60" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9349,7 +9361,7 @@
         <v>800</v>
       </c>
       <c r="P20" s="60" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9357,7 +9369,7 @@
         <v>900</v>
       </c>
       <c r="P21" s="60" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.25">
@@ -9365,7 +9377,7 @@
         <v>1000</v>
       </c>
       <c r="P22" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.25">
@@ -9469,7 +9481,7 @@
         <v>93</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K1" s="65" t="s">
         <v>94</v>

</xml_diff>